<commit_message>
Adds sla and help links
</commit_message>
<xml_diff>
--- a/src/data/raw-data.xlsx
+++ b/src/data/raw-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCodes\aped\16-serviceDetails\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F7308-CC4A-4AF6-BF11-F94DCC631F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE8C75-C7FD-4AA4-82E9-40537B529243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="736">
   <si>
     <t>serviceCode</t>
   </si>
@@ -2058,6 +2058,225 @@
   </si>
   <si>
     <t>ارائه دستورالعمل و نقشه ساخت تجهیزات و تابلوهای برق</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031465101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031465104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031465105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031465107.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031465108.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031465109.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031465110.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466101.pdf</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031466105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466106.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466107.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031466108.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466109.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031466110.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031466111.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031466114.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031467100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031467101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031467102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031467103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031467105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031977100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031977101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031977103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031978100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031465102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031465104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031465105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031465109.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031465110.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031466103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031466104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031466106.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466108.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466110.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031466111.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031466114.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031467101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031467102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031467103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031467105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031977100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031977101.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031977103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031978100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031979103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031979103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031979104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Help_13031979104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031979105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Help_13031979105.jpg</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031980100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/shenasname13031980100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031980102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031980102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031980103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/ServiceHelp_13031980103.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/sla_13031980104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031980104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/SLA_13031980105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/help_13031980105.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13011987100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13011987107.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13031987104.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13032882100.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13032882102.pdf</t>
+  </si>
+  <si>
+    <t>https://aped.ir/Dorsapax/Data/Sub_0/File/Agreement_13032882103.pdf</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2149,6 +2368,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2458,8 +2678,10 @@
   <dimension ref="A1:AA46"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L27" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33:M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,10 +2816,10 @@
       <c r="K2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" t="s">
         <v>34</v>
       </c>
       <c r="N2" s="4" t="s">
@@ -2671,8 +2893,10 @@
       <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1" t="s">
+      <c r="L3" t="s">
+        <v>663</v>
+      </c>
+      <c r="M3" t="s">
         <v>53</v>
       </c>
       <c r="N3" s="4" t="s">
@@ -2746,8 +2970,11 @@
       <c r="K4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" t="s">
         <v>72</v>
+      </c>
+      <c r="M4" t="s">
+        <v>691</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>73</v>
@@ -2820,10 +3047,10 @@
       <c r="K5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" t="s">
         <v>92</v>
       </c>
       <c r="N5" s="4" t="s">
@@ -2897,8 +3124,12 @@
       <c r="K6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="L6" t="s">
+        <v>664</v>
+      </c>
+      <c r="M6" t="s">
+        <v>692</v>
+      </c>
       <c r="N6" s="4" t="s">
         <v>104</v>
       </c>
@@ -2970,6 +3201,12 @@
       <c r="K7" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L7" t="s">
+        <v>665</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>693</v>
+      </c>
       <c r="N7" s="11" t="s">
         <v>120</v>
       </c>
@@ -3041,6 +3278,12 @@
       <c r="K8" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L8" t="s">
+        <v>666</v>
+      </c>
+      <c r="M8" t="s">
+        <v>671</v>
+      </c>
       <c r="N8" s="11" t="s">
         <v>137</v>
       </c>
@@ -3082,7 +3325,10 @@
       <c r="K9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="L9" t="s">
+        <v>667</v>
+      </c>
+      <c r="M9" t="s">
         <v>144</v>
       </c>
       <c r="N9" s="11" t="s">
@@ -3156,6 +3402,12 @@
       <c r="K10" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L10" t="s">
+        <v>668</v>
+      </c>
+      <c r="M10" t="s">
+        <v>694</v>
+      </c>
       <c r="N10" s="12" t="s">
         <v>163</v>
       </c>
@@ -3227,6 +3479,12 @@
       <c r="K11" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L11" t="s">
+        <v>669</v>
+      </c>
+      <c r="M11" t="s">
+        <v>695</v>
+      </c>
       <c r="N11" s="11" t="s">
         <v>174</v>
       </c>
@@ -3298,8 +3556,12 @@
       <c r="K12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="L12" t="s">
+        <v>670</v>
+      </c>
+      <c r="M12" t="s">
+        <v>696</v>
+      </c>
       <c r="N12" s="13" t="s">
         <v>381</v>
       </c>
@@ -3371,8 +3633,12 @@
       <c r="K13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="L13" t="s">
+        <v>671</v>
+      </c>
+      <c r="M13" t="s">
+        <v>697</v>
+      </c>
       <c r="N13" s="13" t="s">
         <v>601</v>
       </c>
@@ -3434,8 +3700,12 @@
       <c r="K14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="L14" t="s">
+        <v>672</v>
+      </c>
+      <c r="M14" t="s">
+        <v>698</v>
+      </c>
       <c r="N14" s="13" t="s">
         <v>419</v>
       </c>
@@ -3507,8 +3777,12 @@
       <c r="K15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="L15" t="s">
+        <v>673</v>
+      </c>
+      <c r="M15" t="s">
+        <v>699</v>
+      </c>
       <c r="N15" s="13" t="s">
         <v>414</v>
       </c>
@@ -3570,8 +3844,12 @@
       <c r="K16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="L16" t="s">
+        <v>674</v>
+      </c>
+      <c r="M16" t="s">
+        <v>700</v>
+      </c>
       <c r="N16" s="13" t="s">
         <v>282</v>
       </c>
@@ -3649,8 +3927,12 @@
       <c r="K17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="L17" t="s">
+        <v>675</v>
+      </c>
+      <c r="M17" t="s">
+        <v>701</v>
+      </c>
       <c r="N17" s="13" t="s">
         <v>315</v>
       </c>
@@ -3712,8 +3994,12 @@
       <c r="K18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="L18" t="s">
+        <v>676</v>
+      </c>
+      <c r="M18" t="s">
+        <v>671</v>
+      </c>
       <c r="N18" s="13" t="s">
         <v>396</v>
       </c>
@@ -3775,8 +4061,12 @@
       <c r="K19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="L19" t="s">
+        <v>677</v>
+      </c>
+      <c r="M19" t="s">
+        <v>702</v>
+      </c>
       <c r="N19" s="13" t="s">
         <v>349</v>
       </c>
@@ -3848,8 +4138,12 @@
       <c r="K20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="L20" t="s">
+        <v>678</v>
+      </c>
+      <c r="M20" t="s">
+        <v>671</v>
+      </c>
       <c r="N20" s="13" t="s">
         <v>298</v>
       </c>
@@ -3927,8 +4221,12 @@
       <c r="K21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="L21" t="s">
+        <v>679</v>
+      </c>
+      <c r="M21" t="s">
+        <v>703</v>
+      </c>
       <c r="N21" s="13" t="s">
         <v>552</v>
       </c>
@@ -3990,8 +4288,12 @@
       <c r="K22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="L22" t="s">
+        <v>680</v>
+      </c>
+      <c r="M22" t="s">
+        <v>704</v>
+      </c>
       <c r="N22" s="13" t="s">
         <v>623</v>
       </c>
@@ -4063,8 +4365,12 @@
       <c r="K23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="L23" t="s">
+        <v>681</v>
+      </c>
+      <c r="M23" t="s">
+        <v>705</v>
+      </c>
       <c r="N23" s="13" t="s">
         <v>310</v>
       </c>
@@ -4126,8 +4432,12 @@
       <c r="K24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="L24" t="s">
+        <v>682</v>
+      </c>
+      <c r="M24" t="s">
+        <v>671</v>
+      </c>
       <c r="N24" s="13" t="s">
         <v>320</v>
       </c>
@@ -4199,8 +4509,12 @@
       <c r="K25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="L25" t="s">
+        <v>683</v>
+      </c>
+      <c r="M25" t="s">
+        <v>706</v>
+      </c>
       <c r="N25" s="13" t="s">
         <v>558</v>
       </c>
@@ -4272,8 +4586,12 @@
       <c r="K26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
+      <c r="L26" t="s">
+        <v>684</v>
+      </c>
+      <c r="M26" t="s">
+        <v>707</v>
+      </c>
       <c r="N26" s="13" t="s">
         <v>335</v>
       </c>
@@ -4345,8 +4663,12 @@
       <c r="K27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
+      <c r="L27" t="s">
+        <v>685</v>
+      </c>
+      <c r="M27" t="s">
+        <v>708</v>
+      </c>
       <c r="N27" s="13" t="s">
         <v>401</v>
       </c>
@@ -4418,8 +4740,12 @@
       <c r="K28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
+      <c r="L28" t="s">
+        <v>686</v>
+      </c>
+      <c r="M28" t="s">
+        <v>709</v>
+      </c>
       <c r="N28" s="13" t="s">
         <v>571</v>
       </c>
@@ -4491,8 +4817,12 @@
       <c r="K29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="L29" t="s">
+        <v>687</v>
+      </c>
+      <c r="M29" t="s">
+        <v>710</v>
+      </c>
       <c r="N29" s="13" t="s">
         <v>475</v>
       </c>
@@ -4564,8 +4894,12 @@
       <c r="K30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="L30" t="s">
+        <v>688</v>
+      </c>
+      <c r="M30" t="s">
+        <v>711</v>
+      </c>
       <c r="N30" s="13" t="s">
         <v>442</v>
       </c>
@@ -4627,8 +4961,12 @@
       <c r="K31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="L31" t="s">
+        <v>689</v>
+      </c>
+      <c r="M31" t="s">
+        <v>712</v>
+      </c>
       <c r="N31" s="13" t="s">
         <v>448</v>
       </c>
@@ -4700,8 +5038,12 @@
       <c r="K32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
+      <c r="L32" t="s">
+        <v>690</v>
+      </c>
+      <c r="M32" t="s">
+        <v>713</v>
+      </c>
       <c r="N32" s="13" t="s">
         <v>491</v>
       </c>
@@ -4773,8 +5115,12 @@
       <c r="K33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="L33" t="s">
+        <v>714</v>
+      </c>
+      <c r="M33" t="s">
+        <v>715</v>
+      </c>
       <c r="N33" s="13" t="s">
         <v>607</v>
       </c>
@@ -4846,8 +5192,12 @@
       <c r="K34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
+      <c r="L34" t="s">
+        <v>716</v>
+      </c>
+      <c r="M34" t="s">
+        <v>717</v>
+      </c>
       <c r="N34" s="13" t="s">
         <v>229</v>
       </c>
@@ -4919,8 +5269,12 @@
       <c r="K35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="L35" t="s">
+        <v>718</v>
+      </c>
+      <c r="M35" t="s">
+        <v>719</v>
+      </c>
       <c r="N35" s="13" t="s">
         <v>253</v>
       </c>
@@ -4998,8 +5352,12 @@
       <c r="K36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
+      <c r="L36" t="s">
+        <v>720</v>
+      </c>
+      <c r="M36" t="s">
+        <v>721</v>
+      </c>
       <c r="N36" s="13" t="s">
         <v>435</v>
       </c>
@@ -5061,8 +5419,12 @@
       <c r="K37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="L37" t="s">
+        <v>722</v>
+      </c>
+      <c r="M37" t="s">
+        <v>723</v>
+      </c>
       <c r="N37" s="13" t="s">
         <v>269</v>
       </c>
@@ -5124,8 +5486,12 @@
       <c r="K38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="L38" t="s">
+        <v>724</v>
+      </c>
+      <c r="M38" t="s">
+        <v>725</v>
+      </c>
       <c r="N38" s="13" t="s">
         <v>459</v>
       </c>
@@ -5197,8 +5563,12 @@
       <c r="K39" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
+      <c r="L39" t="s">
+        <v>726</v>
+      </c>
+      <c r="M39" t="s">
+        <v>727</v>
+      </c>
       <c r="N39" s="13" t="s">
         <v>520</v>
       </c>
@@ -5270,8 +5640,12 @@
       <c r="K40" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
+      <c r="L40" t="s">
+        <v>728</v>
+      </c>
+      <c r="M40" t="s">
+        <v>729</v>
+      </c>
       <c r="N40" s="13" t="s">
         <v>507</v>
       </c>
@@ -5343,8 +5717,12 @@
       <c r="K41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
+      <c r="L41" t="s">
+        <v>730</v>
+      </c>
+      <c r="M41" t="s">
+        <v>671</v>
+      </c>
       <c r="N41" s="13" t="s">
         <v>244</v>
       </c>
@@ -5406,8 +5784,12 @@
       <c r="K42" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
+      <c r="L42" t="s">
+        <v>731</v>
+      </c>
+      <c r="M42" t="s">
+        <v>671</v>
+      </c>
       <c r="N42" s="13" t="s">
         <v>275</v>
       </c>
@@ -5469,8 +5851,12 @@
       <c r="K43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
+      <c r="L43" t="s">
+        <v>732</v>
+      </c>
+      <c r="M43" t="s">
+        <v>671</v>
+      </c>
       <c r="N43" s="13" t="s">
         <v>212</v>
       </c>
@@ -5540,8 +5926,12 @@
       <c r="K44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L44" s="13"/>
-      <c r="M44"/>
+      <c r="L44" t="s">
+        <v>733</v>
+      </c>
+      <c r="M44" t="s">
+        <v>671</v>
+      </c>
       <c r="N44" s="13" t="s">
         <v>536</v>
       </c>
@@ -5613,8 +6003,12 @@
       <c r="K45" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L45" s="13"/>
-      <c r="M45"/>
+      <c r="L45" t="s">
+        <v>734</v>
+      </c>
+      <c r="M45" t="s">
+        <v>671</v>
+      </c>
       <c r="N45" s="13" t="s">
         <v>586</v>
       </c>
@@ -5686,8 +6080,12 @@
       <c r="K46" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L46" s="13"/>
-      <c r="M46"/>
+      <c r="L46" t="s">
+        <v>735</v>
+      </c>
+      <c r="M46" t="s">
+        <v>671</v>
+      </c>
       <c r="N46" s="13" t="s">
         <v>365</v>
       </c>
@@ -5799,8 +6197,9 @@
     <hyperlink ref="O13" r:id="rId70" xr:uid="{20A41675-C1EE-4573-BACC-67D2E6B031F9}"/>
     <hyperlink ref="N44" r:id="rId71" xr:uid="{AB79846E-8255-41E4-B241-AA35E333E9C4}"/>
     <hyperlink ref="O44" r:id="rId72" xr:uid="{726CE31D-826F-4BDB-A66B-D27103C75F65}"/>
+    <hyperlink ref="M7" r:id="rId73" xr:uid="{195590D7-45DA-457D-9931-9804EC87DD90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId73"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds some contact info and corrects question section
</commit_message>
<xml_diff>
--- a/src/data/raw-data.xlsx
+++ b/src/data/raw-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyCodes\aped\16-serviceDetails\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE2FDD3-F7E2-4F0D-A71B-78F10FFF14FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA23CBD-2A8D-4E46-BC89-2433F401A024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="737">
   <si>
     <t>serviceCode</t>
   </si>
@@ -704,9 +704,6 @@
   </si>
   <si>
     <t>آنلاین</t>
-  </si>
-  <si>
-    <t>معاونت بهره برداری - دفتر بازار برق</t>
   </si>
   <si>
     <t>داشتن نام کاربری و کلمه عبور</t>
@@ -1374,9 +1371,6 @@
   </si>
   <si>
     <t>With this service, all subscribers who request the relocation of equipment or whose property is located in the area of power lines can apply for the removal of the area to change the scope of the line.</t>
-  </si>
-  <si>
-    <t>معاونت بهره برداری - معاونت مهندسی</t>
   </si>
   <si>
     <t>https://khadamat.mardom.ir/Service/Details?ServiceId=13031977103</t>
@@ -2274,6 +2268,18 @@
   </si>
   <si>
     <t>121</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> معاونت فروش و خدمات مشترکین - دفتر نظارت بر فروش و وصول مطالبات --واحد مربوطه</t>
+  </si>
+  <si>
+    <t>واحد مربوطه</t>
+  </si>
+  <si>
+    <t>33232612-8</t>
+  </si>
+  <si>
+    <t>معاونت بهره برداری</t>
   </si>
 </sst>
 </file>
@@ -2671,10 +2677,10 @@
   <dimension ref="A1:AA46"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2704,7 @@
     <col min="17" max="25" width="14.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13031465100</v>
       </c>
@@ -2792,16 +2798,16 @@
         <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>30</v>
@@ -2852,7 +2858,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13031465101</v>
       </c>
@@ -2869,16 +2875,16 @@
         <v>49</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>30</v>
@@ -2887,7 +2893,7 @@
         <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="M3" t="s">
         <v>51</v>
@@ -2929,7 +2935,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13031465102</v>
       </c>
@@ -2946,16 +2952,16 @@
         <v>67</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>69</v>
@@ -2967,7 +2973,7 @@
         <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>71</v>
@@ -3006,7 +3012,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13031465103</v>
       </c>
@@ -3023,16 +3029,16 @@
         <v>86</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>87</v>
@@ -3053,10 +3059,10 @@
         <v>203</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>91</v>
@@ -3065,10 +3071,10 @@
         <v>92</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>93</v>
@@ -3077,13 +3083,13 @@
         <v>94</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13031465104</v>
       </c>
@@ -3100,16 +3106,16 @@
         <v>98</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>100</v>
@@ -3118,10 +3124,10 @@
         <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="M6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>101</v>
@@ -3160,7 +3166,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13031465105</v>
       </c>
@@ -3177,16 +3183,16 @@
         <v>116</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>30</v>
@@ -3195,10 +3201,10 @@
         <v>31</v>
       </c>
       <c r="L7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>117</v>
@@ -3237,7 +3243,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13031465107</v>
       </c>
@@ -3254,16 +3260,16 @@
         <v>132</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>133</v>
@@ -3272,10 +3278,10 @@
         <v>31</v>
       </c>
       <c r="L8" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="M8" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N8" s="10" t="s">
         <v>134</v>
@@ -3284,7 +3290,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13031465108</v>
       </c>
@@ -3301,16 +3307,16 @@
         <v>139</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>140</v>
@@ -3319,7 +3325,7 @@
         <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="M9" t="s">
         <v>141</v>
@@ -3361,7 +3367,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13031465109</v>
       </c>
@@ -3378,16 +3384,16 @@
         <v>157</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>158</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>159</v>
@@ -3396,10 +3402,10 @@
         <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="M10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N10" s="11" t="s">
         <v>160</v>
@@ -3438,7 +3444,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13031465110</v>
       </c>
@@ -3455,7 +3461,7 @@
         <v>167</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>168</v>
@@ -3463,8 +3469,8 @@
       <c r="H11" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="I11" s="9">
-        <v>1521</v>
+      <c r="I11" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>170</v>
@@ -3473,10 +3479,10 @@
         <v>31</v>
       </c>
       <c r="L11" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="M11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N11" s="10" t="s">
         <v>171</v>
@@ -3515,33 +3521,33 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13031466101</v>
       </c>
       <c r="B12" t="s">
+        <v>373</v>
+      </c>
+      <c r="C12" t="s">
         <v>374</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>375</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>376</v>
       </c>
-      <c r="E12" t="s">
-        <v>377</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G12" t="s">
         <v>99</v>
       </c>
       <c r="H12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J12" t="s">
         <v>30</v>
@@ -3550,75 +3556,75 @@
         <v>31</v>
       </c>
       <c r="L12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="M12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="N12" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" t="s">
         <v>379</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
+        <v>384</v>
+      </c>
+      <c r="R12" t="s">
         <v>380</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
+        <v>385</v>
+      </c>
+      <c r="T12" t="s">
         <v>381</v>
       </c>
-      <c r="R12" t="s">
+      <c r="U12" t="s">
+        <v>386</v>
+      </c>
+      <c r="V12" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="S12" t="s">
+      <c r="W12" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="X12" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="T12" t="s">
-        <v>384</v>
-      </c>
-      <c r="U12" t="s">
-        <v>385</v>
-      </c>
-      <c r="V12" t="s">
-        <v>386</v>
-      </c>
-      <c r="W12" t="s">
-        <v>387</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>388</v>
       </c>
-      <c r="Y12" t="s">
-        <v>389</v>
-      </c>
     </row>
-    <row r="13" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13031466102</v>
       </c>
       <c r="B13" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C13" t="s">
+        <v>592</v>
+      </c>
+      <c r="D13" t="s">
+        <v>593</v>
+      </c>
+      <c r="E13" t="s">
         <v>594</v>
       </c>
-      <c r="D13" t="s">
-        <v>595</v>
-      </c>
-      <c r="E13" t="s">
-        <v>596</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G13" t="s">
         <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>278</v>
-      </c>
-      <c r="I13" s="9">
-        <v>1521</v>
+        <v>277</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J13" t="s">
         <v>30</v>
@@ -3627,39 +3633,29 @@
         <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="M13" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>598</v>
-      </c>
-      <c r="P13" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>244</v>
-      </c>
-      <c r="R13" t="s">
-        <v>245</v>
-      </c>
-      <c r="S13" t="s">
-        <v>246</v>
-      </c>
-      <c r="T13" t="s">
-        <v>215</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
       <c r="U13"/>
       <c r="V13"/>
       <c r="W13"/>
       <c r="X13"/>
       <c r="Y13"/>
     </row>
-    <row r="14" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13031466103</v>
       </c>
@@ -3667,25 +3663,25 @@
         <v>182</v>
       </c>
       <c r="C14" t="s">
+        <v>412</v>
+      </c>
+      <c r="D14" t="s">
         <v>413</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>414</v>
       </c>
-      <c r="E14" t="s">
-        <v>415</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G14" t="s">
         <v>158</v>
       </c>
       <c r="H14" t="s">
-        <v>278</v>
-      </c>
-      <c r="I14" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J14" t="s">
         <v>30</v>
@@ -3694,75 +3690,75 @@
         <v>31</v>
       </c>
       <c r="L14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="M14" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="N14" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="O14" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="P14" t="s">
         <v>417</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>418</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>419</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>420</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>421</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>422</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>423</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>424</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y14" t="s">
         <v>425</v>
       </c>
-      <c r="X14" t="s">
-        <v>405</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>426</v>
-      </c>
     </row>
-    <row r="15" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13031466104</v>
       </c>
       <c r="B15" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C15" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" t="s">
         <v>408</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>409</v>
       </c>
-      <c r="E15" t="s">
-        <v>410</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G15" t="s">
         <v>158</v>
       </c>
       <c r="H15" t="s">
-        <v>278</v>
-      </c>
-      <c r="I15" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J15" t="s">
         <v>30</v>
@@ -3771,39 +3767,29 @@
         <v>31</v>
       </c>
       <c r="L15" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="M15" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="N15" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="O15" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="O15" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="P15" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>244</v>
-      </c>
-      <c r="R15" t="s">
-        <v>245</v>
-      </c>
-      <c r="S15" t="s">
-        <v>246</v>
-      </c>
-      <c r="T15" t="s">
-        <v>215</v>
-      </c>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
       <c r="U15"/>
       <c r="V15"/>
       <c r="W15"/>
       <c r="X15"/>
       <c r="Y15"/>
     </row>
-    <row r="16" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13031466105</v>
       </c>
@@ -3811,25 +3797,25 @@
         <v>183</v>
       </c>
       <c r="C16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" t="s">
         <v>274</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>275</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G16" t="s">
         <v>276</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G16" t="s">
-        <v>277</v>
-      </c>
       <c r="H16" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J16" t="s">
         <v>30</v>
@@ -3838,52 +3824,46 @@
         <v>31</v>
       </c>
       <c r="L16" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="M16" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="N16" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="O16" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="O16" s="12" t="s">
+      <c r="P16" t="s">
         <v>280</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
+        <v>285</v>
+      </c>
+      <c r="R16" t="s">
         <v>281</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
+        <v>286</v>
+      </c>
+      <c r="T16" t="s">
         <v>282</v>
       </c>
-      <c r="R16" t="s">
+      <c r="U16" t="s">
+        <v>287</v>
+      </c>
+      <c r="V16" t="s">
         <v>283</v>
-      </c>
-      <c r="S16" t="s">
-        <v>284</v>
-      </c>
-      <c r="T16" t="s">
-        <v>285</v>
-      </c>
-      <c r="U16" t="s">
-        <v>286</v>
-      </c>
-      <c r="V16" t="s">
-        <v>287</v>
       </c>
       <c r="W16" t="s">
         <v>288</v>
       </c>
       <c r="X16" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y16" t="s">
         <v>289</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>290</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>289</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
@@ -3894,25 +3874,25 @@
         <v>184</v>
       </c>
       <c r="C17" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" t="s">
         <v>309</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>310</v>
       </c>
-      <c r="E17" t="s">
-        <v>311</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H17" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J17" t="s">
         <v>30</v>
@@ -3921,32 +3901,22 @@
         <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M17" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="N17" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="O17" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="P17" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>244</v>
-      </c>
-      <c r="R17" t="s">
-        <v>245</v>
-      </c>
-      <c r="S17" t="s">
-        <v>246</v>
-      </c>
-      <c r="T17" t="s">
-        <v>215</v>
-      </c>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
       <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
@@ -3961,59 +3931,49 @@
         <v>185</v>
       </c>
       <c r="C18" t="s">
+        <v>389</v>
+      </c>
+      <c r="D18" t="s">
         <v>390</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>391</v>
       </c>
-      <c r="E18" t="s">
-        <v>392</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G18" t="s">
         <v>158</v>
       </c>
       <c r="H18" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L18" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="M18" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N18" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="O18" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="O18" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="P18" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>244</v>
-      </c>
-      <c r="R18" t="s">
-        <v>245</v>
-      </c>
-      <c r="S18" t="s">
-        <v>246</v>
-      </c>
-      <c r="T18" t="s">
-        <v>215</v>
-      </c>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
@@ -4028,16 +3988,16 @@
         <v>186</v>
       </c>
       <c r="C19" t="s">
+        <v>342</v>
+      </c>
+      <c r="D19" t="s">
         <v>343</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>344</v>
       </c>
-      <c r="E19" t="s">
-        <v>345</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G19" t="s">
         <v>158</v>
@@ -4045,8 +4005,8 @@
       <c r="H19" t="s">
         <v>169</v>
       </c>
-      <c r="I19" s="9">
-        <v>1521</v>
+      <c r="I19" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J19" t="s">
         <v>30</v>
@@ -4055,46 +4015,46 @@
         <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="M19" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="N19" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="O19" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="O19" s="12" t="s">
+      <c r="P19" t="s">
         <v>347</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
+        <v>352</v>
+      </c>
+      <c r="R19" t="s">
         <v>348</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="S19" t="s">
+        <v>353</v>
+      </c>
+      <c r="T19" t="s">
         <v>349</v>
       </c>
-      <c r="R19" t="s">
+      <c r="U19" t="s">
+        <v>354</v>
+      </c>
+      <c r="V19" t="s">
         <v>350</v>
-      </c>
-      <c r="S19" t="s">
-        <v>351</v>
-      </c>
-      <c r="T19" t="s">
-        <v>352</v>
-      </c>
-      <c r="U19" t="s">
-        <v>353</v>
-      </c>
-      <c r="V19" t="s">
-        <v>354</v>
       </c>
       <c r="W19" t="s">
         <v>355</v>
       </c>
       <c r="X19" t="s">
+        <v>351</v>
+      </c>
+      <c r="Y19" t="s">
         <v>356</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -4105,25 +4065,25 @@
         <v>187</v>
       </c>
       <c r="C20" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" t="s">
         <v>291</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>292</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G20" t="s">
         <v>293</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G20" t="s">
-        <v>294</v>
       </c>
       <c r="H20" t="s">
         <v>169</v>
       </c>
-      <c r="I20" s="9">
-        <v>1521</v>
+      <c r="I20" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J20" t="s">
         <v>30</v>
@@ -4132,52 +4092,52 @@
         <v>31</v>
       </c>
       <c r="L20" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="M20" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N20" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="O20" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="O20" s="12" t="s">
+      <c r="P20" t="s">
         <v>296</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
+        <v>301</v>
+      </c>
+      <c r="R20" t="s">
         <v>297</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
+        <v>301</v>
+      </c>
+      <c r="T20" t="s">
         <v>298</v>
       </c>
-      <c r="R20" t="s">
+      <c r="U20" t="s">
+        <v>301</v>
+      </c>
+      <c r="V20" t="s">
         <v>299</v>
       </c>
-      <c r="S20" t="s">
+      <c r="W20" t="s">
+        <v>301</v>
+      </c>
+      <c r="X20" t="s">
         <v>300</v>
       </c>
-      <c r="T20" t="s">
+      <c r="Y20" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z20" t="s">
         <v>301</v>
       </c>
-      <c r="U20" t="s">
+      <c r="AA20" t="s">
         <v>302</v>
-      </c>
-      <c r="V20" t="s">
-        <v>302</v>
-      </c>
-      <c r="W20" t="s">
-        <v>302</v>
-      </c>
-      <c r="X20" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>303</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>302</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4188,25 +4148,25 @@
         <v>188</v>
       </c>
       <c r="C21" t="s">
+        <v>542</v>
+      </c>
+      <c r="D21" t="s">
+        <v>543</v>
+      </c>
+      <c r="E21" t="s">
         <v>544</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G21" t="s">
         <v>545</v>
       </c>
-      <c r="E21" t="s">
-        <v>546</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G21" t="s">
-        <v>547</v>
-      </c>
       <c r="H21" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
@@ -4215,32 +4175,22 @@
         <v>31</v>
       </c>
       <c r="L21" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M21" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>549</v>
-      </c>
-      <c r="P21" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>244</v>
-      </c>
-      <c r="R21" t="s">
-        <v>245</v>
-      </c>
-      <c r="S21" t="s">
-        <v>246</v>
-      </c>
-      <c r="T21" t="s">
-        <v>215</v>
-      </c>
+        <v>547</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
@@ -4255,25 +4205,25 @@
         <v>189</v>
       </c>
       <c r="C22" t="s">
+        <v>613</v>
+      </c>
+      <c r="D22" t="s">
+        <v>614</v>
+      </c>
+      <c r="E22" t="s">
         <v>615</v>
       </c>
-      <c r="D22" t="s">
-        <v>616</v>
-      </c>
-      <c r="E22" t="s">
-        <v>617</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G22" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H22" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J22" t="s">
         <v>30</v>
@@ -4282,46 +4232,46 @@
         <v>31</v>
       </c>
       <c r="L22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="M22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="N22" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="P22" t="s">
         <v>618</v>
       </c>
-      <c r="O22" s="12" t="s">
+      <c r="Q22" t="s">
+        <v>623</v>
+      </c>
+      <c r="R22" t="s">
         <v>619</v>
       </c>
-      <c r="P22" t="s">
+      <c r="S22" t="s">
+        <v>624</v>
+      </c>
+      <c r="T22" t="s">
         <v>620</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>621</v>
-      </c>
-      <c r="R22" t="s">
-        <v>622</v>
-      </c>
-      <c r="S22" t="s">
-        <v>623</v>
-      </c>
-      <c r="T22" t="s">
-        <v>624</v>
       </c>
       <c r="U22" t="s">
         <v>625</v>
       </c>
       <c r="V22" t="s">
+        <v>621</v>
+      </c>
+      <c r="W22" t="s">
         <v>626</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y22" t="s">
         <v>627</v>
-      </c>
-      <c r="X22" t="s">
-        <v>628</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
@@ -4329,19 +4279,19 @@
         <v>13031466114</v>
       </c>
       <c r="B23" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C23" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" t="s">
         <v>304</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>305</v>
       </c>
-      <c r="E23" t="s">
-        <v>306</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G23" t="s">
         <v>50</v>
@@ -4349,8 +4299,8 @@
       <c r="H23" t="s">
         <v>169</v>
       </c>
-      <c r="I23" s="9">
-        <v>1521</v>
+      <c r="I23" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J23" t="s">
         <v>30</v>
@@ -4359,32 +4309,22 @@
         <v>31</v>
       </c>
       <c r="L23" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M23" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="N23" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="P23" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>244</v>
-      </c>
-      <c r="R23" t="s">
-        <v>245</v>
-      </c>
-      <c r="S23" t="s">
-        <v>246</v>
-      </c>
-      <c r="T23" t="s">
-        <v>215</v>
-      </c>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
       <c r="U23"/>
       <c r="V23"/>
       <c r="W23"/>
@@ -4399,73 +4339,73 @@
         <v>190</v>
       </c>
       <c r="C24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" t="s">
         <v>314</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>315</v>
       </c>
-      <c r="E24" t="s">
-        <v>316</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G24" t="s">
         <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>278</v>
-      </c>
-      <c r="I24" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L24" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="M24" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N24" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="O24" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="O24" s="12" t="s">
+      <c r="P24" t="s">
         <v>318</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
+        <v>323</v>
+      </c>
+      <c r="R24" t="s">
         <v>319</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="S24" t="s">
+        <v>324</v>
+      </c>
+      <c r="T24" t="s">
         <v>320</v>
       </c>
-      <c r="R24" t="s">
+      <c r="U24" t="s">
+        <v>325</v>
+      </c>
+      <c r="V24" t="s">
         <v>321</v>
-      </c>
-      <c r="S24" t="s">
-        <v>322</v>
-      </c>
-      <c r="T24" t="s">
-        <v>323</v>
-      </c>
-      <c r="U24" t="s">
-        <v>324</v>
-      </c>
-      <c r="V24" t="s">
-        <v>325</v>
       </c>
       <c r="W24" t="s">
         <v>326</v>
       </c>
       <c r="X24" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y24" t="s">
         <v>327</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4473,76 +4413,76 @@
         <v>13031467101</v>
       </c>
       <c r="B25" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C25" t="s">
+        <v>548</v>
+      </c>
+      <c r="D25" t="s">
+        <v>549</v>
+      </c>
+      <c r="E25" t="s">
         <v>550</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G25" t="s">
         <v>551</v>
       </c>
-      <c r="E25" t="s">
-        <v>552</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G25" t="s">
-        <v>553</v>
-      </c>
       <c r="H25" t="s">
-        <v>278</v>
-      </c>
-      <c r="I25" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="M25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="N25" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="P25" t="s">
         <v>554</v>
       </c>
-      <c r="O25" s="12" t="s">
+      <c r="Q25" t="s">
+        <v>559</v>
+      </c>
+      <c r="R25" t="s">
         <v>555</v>
       </c>
-      <c r="P25" t="s">
+      <c r="S25" t="s">
+        <v>405</v>
+      </c>
+      <c r="T25" t="s">
         <v>556</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="U25" t="s">
+        <v>405</v>
+      </c>
+      <c r="V25" t="s">
         <v>557</v>
       </c>
-      <c r="R25" t="s">
+      <c r="W25" t="s">
+        <v>560</v>
+      </c>
+      <c r="X25" t="s">
         <v>558</v>
       </c>
-      <c r="S25" t="s">
-        <v>559</v>
-      </c>
-      <c r="T25" t="s">
-        <v>560</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="Y25" t="s">
         <v>561</v>
-      </c>
-      <c r="V25" t="s">
-        <v>406</v>
-      </c>
-      <c r="W25" t="s">
-        <v>406</v>
-      </c>
-      <c r="X25" t="s">
-        <v>562</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="45" x14ac:dyDescent="0.25">
@@ -4550,76 +4490,76 @@
         <v>13031467102</v>
       </c>
       <c r="B26" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C26" t="s">
+        <v>328</v>
+      </c>
+      <c r="D26" t="s">
         <v>329</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>330</v>
       </c>
-      <c r="E26" t="s">
-        <v>331</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G26" t="s">
         <v>158</v>
       </c>
       <c r="H26" t="s">
-        <v>278</v>
-      </c>
-      <c r="I26" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L26" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M26" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="N26" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="O26" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="O26" s="12" t="s">
+      <c r="P26" t="s">
         <v>333</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
+        <v>338</v>
+      </c>
+      <c r="R26" t="s">
         <v>334</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="S26" t="s">
+        <v>339</v>
+      </c>
+      <c r="T26" t="s">
         <v>335</v>
       </c>
-      <c r="R26" t="s">
+      <c r="U26" t="s">
+        <v>340</v>
+      </c>
+      <c r="V26" t="s">
         <v>336</v>
-      </c>
-      <c r="S26" t="s">
-        <v>337</v>
-      </c>
-      <c r="T26" t="s">
-        <v>338</v>
-      </c>
-      <c r="U26" t="s">
-        <v>339</v>
-      </c>
-      <c r="V26" t="s">
-        <v>340</v>
       </c>
       <c r="W26" t="s">
         <v>341</v>
       </c>
       <c r="X26" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="Y26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -4630,73 +4570,73 @@
         <v>191</v>
       </c>
       <c r="C27" t="s">
+        <v>394</v>
+      </c>
+      <c r="D27" t="s">
         <v>395</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>396</v>
       </c>
-      <c r="E27" t="s">
-        <v>397</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G27" t="s">
         <v>158</v>
       </c>
       <c r="H27" t="s">
-        <v>278</v>
-      </c>
-      <c r="I27" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J27" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L27" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="M27" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="N27" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="O27" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="O27" s="12" t="s">
+      <c r="P27" t="s">
         <v>399</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
+        <v>404</v>
+      </c>
+      <c r="R27" t="s">
         <v>400</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="S27" t="s">
+        <v>405</v>
+      </c>
+      <c r="T27" t="s">
         <v>401</v>
       </c>
-      <c r="R27" t="s">
+      <c r="U27" t="s">
+        <v>404</v>
+      </c>
+      <c r="V27" t="s">
         <v>402</v>
       </c>
-      <c r="S27" t="s">
+      <c r="W27" t="s">
+        <v>406</v>
+      </c>
+      <c r="X27" t="s">
         <v>403</v>
       </c>
-      <c r="T27" t="s">
-        <v>404</v>
-      </c>
-      <c r="U27" t="s">
+      <c r="Y27" t="s">
         <v>405</v>
-      </c>
-      <c r="V27" t="s">
-        <v>406</v>
-      </c>
-      <c r="W27" t="s">
-        <v>405</v>
-      </c>
-      <c r="X27" t="s">
-        <v>407</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
@@ -4707,73 +4647,73 @@
         <v>192</v>
       </c>
       <c r="C28" t="s">
+        <v>562</v>
+      </c>
+      <c r="D28" t="s">
+        <v>563</v>
+      </c>
+      <c r="E28" t="s">
         <v>564</v>
       </c>
-      <c r="D28" t="s">
-        <v>565</v>
-      </c>
-      <c r="E28" t="s">
-        <v>566</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G28" t="s">
         <v>158</v>
       </c>
       <c r="H28" t="s">
-        <v>278</v>
-      </c>
-      <c r="I28" s="9">
-        <v>1521</v>
+        <v>733</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>734</v>
       </c>
       <c r="J28" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L28" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="M28" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="N28" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="P28" t="s">
         <v>567</v>
       </c>
-      <c r="O28" s="12" t="s">
+      <c r="Q28" t="s">
+        <v>404</v>
+      </c>
+      <c r="R28" t="s">
         <v>568</v>
-      </c>
-      <c r="P28" t="s">
-        <v>569</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>570</v>
-      </c>
-      <c r="R28" t="s">
-        <v>571</v>
       </c>
       <c r="S28" t="s">
         <v>572</v>
       </c>
       <c r="T28" t="s">
+        <v>569</v>
+      </c>
+      <c r="U28" t="s">
         <v>573</v>
       </c>
-      <c r="U28" t="s">
-        <v>405</v>
-      </c>
       <c r="V28" t="s">
+        <v>570</v>
+      </c>
+      <c r="W28" t="s">
         <v>574</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
+        <v>571</v>
+      </c>
+      <c r="Y28" t="s">
         <v>575</v>
-      </c>
-      <c r="X28" t="s">
-        <v>576</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="29" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4784,73 +4724,73 @@
         <v>193</v>
       </c>
       <c r="C29" t="s">
+        <v>466</v>
+      </c>
+      <c r="D29" t="s">
+        <v>467</v>
+      </c>
+      <c r="E29" t="s">
         <v>468</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G29" t="s">
+        <v>276</v>
+      </c>
+      <c r="H29" t="s">
+        <v>264</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="J29" t="s">
         <v>469</v>
-      </c>
-      <c r="E29" t="s">
-        <v>470</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G29" t="s">
-        <v>277</v>
-      </c>
-      <c r="H29" t="s">
-        <v>265</v>
-      </c>
-      <c r="I29" s="9">
-        <v>1521</v>
-      </c>
-      <c r="J29" t="s">
-        <v>471</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L29" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="M29" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="N29" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="P29" t="s">
         <v>472</v>
       </c>
-      <c r="O29" s="12" t="s">
+      <c r="Q29" t="s">
+        <v>477</v>
+      </c>
+      <c r="R29" t="s">
         <v>473</v>
       </c>
-      <c r="P29" t="s">
+      <c r="S29" t="s">
+        <v>478</v>
+      </c>
+      <c r="T29" t="s">
         <v>474</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>475</v>
-      </c>
-      <c r="R29" t="s">
-        <v>476</v>
-      </c>
-      <c r="S29" t="s">
-        <v>477</v>
-      </c>
-      <c r="T29" t="s">
-        <v>478</v>
       </c>
       <c r="U29" t="s">
         <v>479</v>
       </c>
       <c r="V29" t="s">
+        <v>475</v>
+      </c>
+      <c r="W29" t="s">
         <v>480</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
+        <v>476</v>
+      </c>
+      <c r="Y29" t="s">
         <v>481</v>
-      </c>
-      <c r="X29" t="s">
-        <v>482</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -4861,63 +4801,63 @@
         <v>194</v>
       </c>
       <c r="C30" t="s">
+        <v>433</v>
+      </c>
+      <c r="D30" t="s">
         <v>434</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>435</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G30" t="s">
         <v>436</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
+        <v>264</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="J30" t="s">
         <v>437</v>
-      </c>
-      <c r="H30" t="s">
-        <v>265</v>
-      </c>
-      <c r="I30" s="9">
-        <v>1521</v>
-      </c>
-      <c r="J30" t="s">
-        <v>438</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L30" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="M30" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="N30" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="O30" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="O30" s="12" t="s">
-        <v>440</v>
-      </c>
       <c r="P30" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q30"/>
+      <c r="R30" t="s">
         <v>243</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="S30"/>
+      <c r="T30" t="s">
         <v>244</v>
       </c>
-      <c r="R30" t="s">
+      <c r="U30"/>
+      <c r="V30" t="s">
         <v>245</v>
       </c>
-      <c r="S30" t="s">
-        <v>246</v>
-      </c>
-      <c r="T30" t="s">
+      <c r="W30"/>
+      <c r="X30" t="s">
         <v>215</v>
       </c>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
       <c r="Y30"/>
     </row>
     <row r="31" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4928,73 +4868,73 @@
         <v>195</v>
       </c>
       <c r="C31" t="s">
+        <v>440</v>
+      </c>
+      <c r="D31" t="s">
         <v>441</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>442</v>
       </c>
-      <c r="E31" t="s">
-        <v>443</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G31" t="s">
         <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>444</v>
-      </c>
-      <c r="I31" s="9">
-        <v>1521</v>
+        <v>736</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>735</v>
       </c>
       <c r="J31" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L31" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="M31" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="N31" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="P31" t="s">
         <v>445</v>
       </c>
-      <c r="O31" s="12" t="s">
+      <c r="Q31" t="s">
+        <v>450</v>
+      </c>
+      <c r="R31" t="s">
         <v>446</v>
-      </c>
-      <c r="P31" t="s">
-        <v>447</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>448</v>
-      </c>
-      <c r="R31" t="s">
-        <v>449</v>
       </c>
       <c r="S31" t="s">
         <v>450</v>
       </c>
       <c r="T31" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="U31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="V31" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="W31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="X31" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="Y31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -5005,73 +4945,73 @@
         <v>196</v>
       </c>
       <c r="C32" t="s">
+        <v>482</v>
+      </c>
+      <c r="D32" t="s">
+        <v>483</v>
+      </c>
+      <c r="E32" t="s">
         <v>484</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G32" t="s">
+        <v>436</v>
+      </c>
+      <c r="H32" t="s">
+        <v>429</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="J32" t="s">
         <v>485</v>
-      </c>
-      <c r="E32" t="s">
-        <v>486</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G32" t="s">
-        <v>437</v>
-      </c>
-      <c r="H32" t="s">
-        <v>430</v>
-      </c>
-      <c r="I32" s="9">
-        <v>1521</v>
-      </c>
-      <c r="J32" t="s">
-        <v>487</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L32" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="M32" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N32" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="P32" t="s">
         <v>488</v>
       </c>
-      <c r="O32" s="12" t="s">
+      <c r="Q32" t="s">
+        <v>493</v>
+      </c>
+      <c r="R32" t="s">
         <v>489</v>
       </c>
-      <c r="P32" t="s">
+      <c r="S32" t="s">
+        <v>494</v>
+      </c>
+      <c r="T32" t="s">
         <v>490</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>491</v>
-      </c>
-      <c r="R32" t="s">
-        <v>492</v>
-      </c>
-      <c r="S32" t="s">
-        <v>493</v>
-      </c>
-      <c r="T32" t="s">
-        <v>494</v>
       </c>
       <c r="U32" t="s">
         <v>495</v>
       </c>
       <c r="V32" t="s">
+        <v>491</v>
+      </c>
+      <c r="W32" t="s">
         <v>496</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
+        <v>492</v>
+      </c>
+      <c r="Y32" t="s">
         <v>497</v>
-      </c>
-      <c r="X32" t="s">
-        <v>498</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
@@ -5079,76 +5019,76 @@
         <v>13031979103</v>
       </c>
       <c r="B33" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C33" t="s">
+        <v>597</v>
+      </c>
+      <c r="D33" t="s">
+        <v>598</v>
+      </c>
+      <c r="E33" t="s">
         <v>599</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G33" t="s">
         <v>600</v>
       </c>
-      <c r="E33" t="s">
-        <v>601</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G33" t="s">
-        <v>602</v>
-      </c>
       <c r="H33" t="s">
-        <v>224</v>
-      </c>
-      <c r="I33" s="9">
-        <v>1521</v>
+        <v>270</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J33" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L33" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="M33" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="N33" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="P33" t="s">
         <v>603</v>
       </c>
-      <c r="O33" s="12" t="s">
+      <c r="Q33" t="s">
+        <v>608</v>
+      </c>
+      <c r="R33" t="s">
         <v>604</v>
       </c>
-      <c r="P33" t="s">
+      <c r="S33" t="s">
+        <v>609</v>
+      </c>
+      <c r="T33" t="s">
         <v>605</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>606</v>
-      </c>
-      <c r="R33" t="s">
-        <v>607</v>
-      </c>
-      <c r="S33" t="s">
-        <v>608</v>
-      </c>
-      <c r="T33" t="s">
-        <v>609</v>
       </c>
       <c r="U33" t="s">
         <v>610</v>
       </c>
       <c r="V33" t="s">
+        <v>606</v>
+      </c>
+      <c r="W33" t="s">
         <v>611</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
+        <v>607</v>
+      </c>
+      <c r="Y33" t="s">
         <v>612</v>
-      </c>
-      <c r="X33" t="s">
-        <v>613</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
@@ -5156,7 +5096,7 @@
         <v>13031979104</v>
       </c>
       <c r="B34" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C34" t="s">
         <v>220</v>
@@ -5168,64 +5108,64 @@
         <v>222</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G34" t="s">
         <v>223</v>
       </c>
       <c r="H34" t="s">
+        <v>270</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="J34" t="s">
         <v>224</v>
-      </c>
-      <c r="I34" s="9">
-        <v>1521</v>
-      </c>
-      <c r="J34" t="s">
-        <v>225</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L34" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="M34" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="N34" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="O34" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="O34" s="12" t="s">
+      <c r="P34" t="s">
         <v>227</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
+        <v>232</v>
+      </c>
+      <c r="R34" t="s">
         <v>228</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="S34" t="s">
+        <v>233</v>
+      </c>
+      <c r="T34" t="s">
         <v>229</v>
       </c>
-      <c r="R34" t="s">
+      <c r="U34" t="s">
+        <v>234</v>
+      </c>
+      <c r="V34" t="s">
         <v>230</v>
-      </c>
-      <c r="S34" t="s">
-        <v>231</v>
-      </c>
-      <c r="T34" t="s">
-        <v>232</v>
-      </c>
-      <c r="U34" t="s">
-        <v>233</v>
-      </c>
-      <c r="V34" t="s">
-        <v>234</v>
       </c>
       <c r="W34" t="s">
         <v>235</v>
       </c>
       <c r="X34" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y34" t="s">
         <v>236</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -5233,82 +5173,82 @@
         <v>13031979105</v>
       </c>
       <c r="B35" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" t="s">
         <v>247</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>248</v>
       </c>
-      <c r="E35" t="s">
-        <v>249</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G35" t="s">
         <v>223</v>
       </c>
       <c r="H35" t="s">
+        <v>270</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="J35" t="s">
         <v>224</v>
-      </c>
-      <c r="I35" s="9">
-        <v>1521</v>
-      </c>
-      <c r="J35" t="s">
-        <v>225</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L35" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="M35" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="N35" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="O35" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="O35" s="12" t="s">
+      <c r="P35" t="s">
         <v>251</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
+        <v>256</v>
+      </c>
+      <c r="R35" t="s">
         <v>252</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="S35" t="s">
+        <v>257</v>
+      </c>
+      <c r="T35" t="s">
         <v>253</v>
       </c>
-      <c r="R35" t="s">
+      <c r="U35" t="s">
+        <v>258</v>
+      </c>
+      <c r="V35" t="s">
         <v>254</v>
-      </c>
-      <c r="S35" t="s">
-        <v>255</v>
-      </c>
-      <c r="T35" t="s">
-        <v>256</v>
-      </c>
-      <c r="U35" t="s">
-        <v>257</v>
-      </c>
-      <c r="V35" t="s">
-        <v>258</v>
       </c>
       <c r="W35" t="s">
         <v>259</v>
       </c>
       <c r="X35" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y35" t="s">
         <v>260</v>
       </c>
-      <c r="Y35" t="s">
-        <v>261</v>
-      </c>
       <c r="Z35" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA35" t="s">
         <v>260</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -5319,63 +5259,63 @@
         <v>197</v>
       </c>
       <c r="C36" t="s">
+        <v>426</v>
+      </c>
+      <c r="D36" t="s">
         <v>427</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>428</v>
       </c>
-      <c r="E36" t="s">
-        <v>429</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G36" t="s">
         <v>99</v>
       </c>
       <c r="H36" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L36" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="M36" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="N36" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="O36" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="O36" s="12" t="s">
-        <v>433</v>
-      </c>
       <c r="P36" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q36"/>
+      <c r="R36" t="s">
         <v>243</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="S36"/>
+      <c r="T36" t="s">
         <v>244</v>
       </c>
-      <c r="R36" t="s">
+      <c r="U36"/>
+      <c r="V36" t="s">
         <v>245</v>
       </c>
-      <c r="S36" t="s">
-        <v>246</v>
-      </c>
-      <c r="T36" t="s">
+      <c r="W36"/>
+      <c r="X36" t="s">
         <v>215</v>
       </c>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
       <c r="Y36"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -5383,66 +5323,66 @@
         <v>13031980102</v>
       </c>
       <c r="B37" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C37" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" t="s">
         <v>262</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>263</v>
       </c>
-      <c r="E37" t="s">
-        <v>264</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G37" t="s">
         <v>50</v>
       </c>
       <c r="H37" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J37" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L37" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="M37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="N37" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="O37" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="O37" s="12" t="s">
-        <v>267</v>
-      </c>
       <c r="P37" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q37"/>
+      <c r="R37" t="s">
         <v>243</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="S37"/>
+      <c r="T37" t="s">
         <v>244</v>
       </c>
-      <c r="R37" t="s">
+      <c r="U37"/>
+      <c r="V37" t="s">
         <v>245</v>
       </c>
-      <c r="S37" t="s">
-        <v>246</v>
-      </c>
-      <c r="T37" t="s">
+      <c r="W37"/>
+      <c r="X37" t="s">
         <v>215</v>
       </c>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
       <c r="Y37"/>
     </row>
     <row r="38" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5450,28 +5390,28 @@
         <v>13031980103</v>
       </c>
       <c r="B38" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C38" t="s">
+        <v>451</v>
+      </c>
+      <c r="D38" t="s">
+        <v>452</v>
+      </c>
+      <c r="E38" t="s">
         <v>453</v>
       </c>
-      <c r="D38" t="s">
-        <v>454</v>
-      </c>
-      <c r="E38" t="s">
-        <v>455</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H38" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J38" t="s">
         <v>30</v>
@@ -5480,46 +5420,46 @@
         <v>31</v>
       </c>
       <c r="L38" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="M38" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="N38" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="P38" t="s">
         <v>456</v>
       </c>
-      <c r="O38" s="12" t="s">
+      <c r="Q38" t="s">
+        <v>461</v>
+      </c>
+      <c r="R38" t="s">
         <v>457</v>
       </c>
-      <c r="P38" t="s">
+      <c r="S38" t="s">
+        <v>462</v>
+      </c>
+      <c r="T38" t="s">
         <v>458</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>459</v>
-      </c>
-      <c r="R38" t="s">
-        <v>460</v>
-      </c>
-      <c r="S38" t="s">
-        <v>461</v>
-      </c>
-      <c r="T38" t="s">
-        <v>462</v>
       </c>
       <c r="U38" t="s">
         <v>463</v>
       </c>
       <c r="V38" t="s">
+        <v>459</v>
+      </c>
+      <c r="W38" t="s">
         <v>464</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
+        <v>460</v>
+      </c>
+      <c r="Y38" t="s">
         <v>465</v>
-      </c>
-      <c r="X38" t="s">
-        <v>466</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
@@ -5530,73 +5470,73 @@
         <v>198</v>
       </c>
       <c r="C39" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D39" t="s">
+        <v>262</v>
+      </c>
+      <c r="E39" t="s">
         <v>263</v>
       </c>
-      <c r="E39" t="s">
-        <v>264</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G39" t="s">
         <v>158</v>
       </c>
       <c r="H39" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J39" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L39" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M39" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="N39" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>515</v>
+      </c>
+      <c r="P39" t="s">
         <v>516</v>
       </c>
-      <c r="O39" s="12" t="s">
+      <c r="Q39" t="s">
+        <v>521</v>
+      </c>
+      <c r="R39" t="s">
         <v>517</v>
       </c>
-      <c r="P39" t="s">
+      <c r="S39" t="s">
+        <v>522</v>
+      </c>
+      <c r="T39" t="s">
         <v>518</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>519</v>
-      </c>
-      <c r="R39" t="s">
-        <v>520</v>
-      </c>
-      <c r="S39" t="s">
-        <v>521</v>
-      </c>
-      <c r="T39" t="s">
-        <v>522</v>
       </c>
       <c r="U39" t="s">
         <v>523</v>
       </c>
       <c r="V39" t="s">
+        <v>519</v>
+      </c>
+      <c r="W39" t="s">
         <v>524</v>
       </c>
-      <c r="W39" t="s">
+      <c r="X39" t="s">
+        <v>520</v>
+      </c>
+      <c r="Y39" t="s">
         <v>525</v>
-      </c>
-      <c r="X39" t="s">
-        <v>526</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -5607,73 +5547,73 @@
         <v>199</v>
       </c>
       <c r="C40" t="s">
+        <v>498</v>
+      </c>
+      <c r="D40" t="s">
+        <v>499</v>
+      </c>
+      <c r="E40" t="s">
         <v>500</v>
       </c>
-      <c r="D40" t="s">
-        <v>501</v>
-      </c>
-      <c r="E40" t="s">
-        <v>502</v>
-      </c>
       <c r="F40" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G40" t="s">
         <v>68</v>
       </c>
       <c r="H40" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J40" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L40" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="M40" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N40" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="P40" t="s">
         <v>503</v>
       </c>
-      <c r="O40" s="12" t="s">
+      <c r="Q40" t="s">
+        <v>508</v>
+      </c>
+      <c r="R40" t="s">
         <v>504</v>
       </c>
-      <c r="P40" t="s">
+      <c r="S40" t="s">
+        <v>509</v>
+      </c>
+      <c r="T40" t="s">
         <v>505</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>506</v>
-      </c>
-      <c r="R40" t="s">
-        <v>507</v>
-      </c>
-      <c r="S40" t="s">
-        <v>508</v>
-      </c>
-      <c r="T40" t="s">
-        <v>509</v>
       </c>
       <c r="U40" t="s">
         <v>510</v>
       </c>
       <c r="V40" t="s">
+        <v>506</v>
+      </c>
+      <c r="W40" t="s">
         <v>511</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
+        <v>507</v>
+      </c>
+      <c r="Y40" t="s">
         <v>512</v>
-      </c>
-      <c r="X40" t="s">
-        <v>513</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -5684,16 +5624,16 @@
         <v>200</v>
       </c>
       <c r="C41" t="s">
+        <v>237</v>
+      </c>
+      <c r="D41" t="s">
         <v>238</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>239</v>
       </c>
-      <c r="E41" t="s">
-        <v>240</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G41" t="s">
         <v>50</v>
@@ -5701,46 +5641,46 @@
       <c r="H41" t="s">
         <v>169</v>
       </c>
-      <c r="I41" s="9">
-        <v>1521</v>
+      <c r="I41" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J41" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L41" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="M41" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N41" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="O41" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="O41" s="12" t="s">
+      <c r="P41" t="s">
         <v>242</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41"/>
+      <c r="R41" t="s">
         <v>243</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="S41"/>
+      <c r="T41" t="s">
         <v>244</v>
       </c>
-      <c r="R41" t="s">
+      <c r="U41"/>
+      <c r="V41" t="s">
         <v>245</v>
       </c>
-      <c r="S41" t="s">
-        <v>246</v>
-      </c>
-      <c r="T41" t="s">
+      <c r="W41"/>
+      <c r="X41" t="s">
         <v>215</v>
       </c>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
       <c r="Y41"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -5751,63 +5691,63 @@
         <v>201</v>
       </c>
       <c r="C42" t="s">
+        <v>267</v>
+      </c>
+      <c r="D42" t="s">
         <v>268</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>269</v>
       </c>
-      <c r="E42" t="s">
-        <v>270</v>
-      </c>
       <c r="F42" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G42" t="s">
         <v>50</v>
       </c>
       <c r="H42" t="s">
-        <v>271</v>
-      </c>
-      <c r="I42" s="9">
-        <v>1521</v>
+        <v>270</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J42" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L42" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="M42" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N42" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="O42" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="O42" s="12" t="s">
-        <v>273</v>
-      </c>
       <c r="P42" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q42"/>
+      <c r="R42" t="s">
         <v>243</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="S42"/>
+      <c r="T42" t="s">
         <v>244</v>
       </c>
-      <c r="R42" t="s">
+      <c r="U42"/>
+      <c r="V42" t="s">
         <v>245</v>
       </c>
-      <c r="S42" t="s">
-        <v>246</v>
-      </c>
-      <c r="T42" t="s">
+      <c r="W42"/>
+      <c r="X42" t="s">
         <v>215</v>
       </c>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-      <c r="X42"/>
       <c r="Y42"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -5815,7 +5755,7 @@
         <v>13031987104</v>
       </c>
       <c r="B43" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C43" t="s">
         <v>205</v>
@@ -5827,7 +5767,7 @@
         <v>207</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G43" t="s">
         <v>50</v>
@@ -5835,20 +5775,20 @@
       <c r="H43" t="s">
         <v>208</v>
       </c>
-      <c r="I43" s="9">
-        <v>1521</v>
+      <c r="I43" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J43" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L43" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="M43" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N43" s="12" t="s">
         <v>209</v>
@@ -5860,28 +5800,28 @@
         <v>211</v>
       </c>
       <c r="Q43" t="s">
+        <v>216</v>
+      </c>
+      <c r="R43" t="s">
         <v>212</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
+        <v>217</v>
+      </c>
+      <c r="T43" t="s">
         <v>213</v>
       </c>
-      <c r="S43" t="s">
+      <c r="U43" t="s">
+        <v>218</v>
+      </c>
+      <c r="V43" t="s">
         <v>214</v>
       </c>
-      <c r="T43" t="s">
+      <c r="W43" t="s">
+        <v>219</v>
+      </c>
+      <c r="X43" t="s">
         <v>215</v>
-      </c>
-      <c r="U43" t="s">
-        <v>216</v>
-      </c>
-      <c r="V43" t="s">
-        <v>217</v>
-      </c>
-      <c r="W43" t="s">
-        <v>218</v>
-      </c>
-      <c r="X43" t="s">
-        <v>219</v>
       </c>
       <c r="Y43"/>
     </row>
@@ -5890,76 +5830,76 @@
         <v>13032882100</v>
       </c>
       <c r="B44" t="s">
+        <v>643</v>
+      </c>
+      <c r="C44" t="s">
+        <v>526</v>
+      </c>
+      <c r="D44" t="s">
+        <v>527</v>
+      </c>
+      <c r="E44" t="s">
+        <v>528</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="C44" t="s">
-        <v>528</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>529</v>
       </c>
-      <c r="E44" t="s">
-        <v>530</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G44" t="s">
-        <v>531</v>
-      </c>
       <c r="H44" t="s">
-        <v>361</v>
-      </c>
-      <c r="I44" s="9">
-        <v>1521</v>
+        <v>360</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J44" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L44" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="M44" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N44" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="P44" t="s">
         <v>532</v>
       </c>
-      <c r="O44" s="12" t="s">
+      <c r="Q44" t="s">
+        <v>537</v>
+      </c>
+      <c r="R44" t="s">
         <v>533</v>
       </c>
-      <c r="P44" t="s">
+      <c r="S44" t="s">
+        <v>538</v>
+      </c>
+      <c r="T44" t="s">
         <v>534</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>535</v>
-      </c>
-      <c r="R44" t="s">
-        <v>536</v>
-      </c>
-      <c r="S44" t="s">
-        <v>537</v>
-      </c>
-      <c r="T44" t="s">
-        <v>538</v>
       </c>
       <c r="U44" t="s">
         <v>539</v>
       </c>
       <c r="V44" t="s">
+        <v>535</v>
+      </c>
+      <c r="W44" t="s">
         <v>540</v>
       </c>
-      <c r="W44" t="s">
+      <c r="X44" t="s">
+        <v>536</v>
+      </c>
+      <c r="Y44" t="s">
         <v>541</v>
-      </c>
-      <c r="X44" t="s">
-        <v>542</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -5970,73 +5910,73 @@
         <v>202</v>
       </c>
       <c r="C45" t="s">
+        <v>576</v>
+      </c>
+      <c r="D45" t="s">
+        <v>577</v>
+      </c>
+      <c r="E45" t="s">
         <v>578</v>
       </c>
-      <c r="D45" t="s">
+      <c r="F45" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G45" t="s">
         <v>579</v>
       </c>
-      <c r="E45" t="s">
-        <v>580</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G45" t="s">
-        <v>581</v>
-      </c>
       <c r="H45" t="s">
-        <v>361</v>
-      </c>
-      <c r="I45" s="9">
-        <v>1521</v>
+        <v>360</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J45" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L45" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="M45" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N45" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="P45" t="s">
         <v>582</v>
       </c>
-      <c r="O45" s="12" t="s">
+      <c r="Q45" t="s">
+        <v>587</v>
+      </c>
+      <c r="R45" t="s">
         <v>583</v>
       </c>
-      <c r="P45" t="s">
+      <c r="S45" t="s">
+        <v>588</v>
+      </c>
+      <c r="T45" t="s">
         <v>584</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>585</v>
-      </c>
-      <c r="R45" t="s">
-        <v>586</v>
-      </c>
-      <c r="S45" t="s">
-        <v>587</v>
-      </c>
-      <c r="T45" t="s">
-        <v>588</v>
       </c>
       <c r="U45" t="s">
         <v>589</v>
       </c>
       <c r="V45" t="s">
+        <v>585</v>
+      </c>
+      <c r="W45" t="s">
         <v>590</v>
       </c>
-      <c r="W45" t="s">
+      <c r="X45" t="s">
+        <v>586</v>
+      </c>
+      <c r="Y45" t="s">
         <v>591</v>
-      </c>
-      <c r="X45" t="s">
-        <v>592</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -6044,76 +5984,76 @@
         <v>13032882103</v>
       </c>
       <c r="B46" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C46" t="s">
+        <v>357</v>
+      </c>
+      <c r="D46" t="s">
         <v>358</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>359</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G46" t="s">
+        <v>293</v>
+      </c>
+      <c r="H46" t="s">
         <v>360</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="G46" t="s">
-        <v>294</v>
-      </c>
-      <c r="H46" t="s">
-        <v>361</v>
-      </c>
-      <c r="I46" s="9">
-        <v>1521</v>
+      <c r="I46" s="9" t="s">
+        <v>730</v>
       </c>
       <c r="J46" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L46" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="M46" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N46" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="O46" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="O46" s="12" t="s">
+      <c r="P46" t="s">
         <v>363</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
+        <v>368</v>
+      </c>
+      <c r="R46" t="s">
         <v>364</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="S46" t="s">
+        <v>369</v>
+      </c>
+      <c r="T46" t="s">
         <v>365</v>
       </c>
-      <c r="R46" t="s">
+      <c r="U46" t="s">
+        <v>370</v>
+      </c>
+      <c r="V46" t="s">
         <v>366</v>
-      </c>
-      <c r="S46" t="s">
-        <v>367</v>
-      </c>
-      <c r="T46" t="s">
-        <v>368</v>
-      </c>
-      <c r="U46" t="s">
-        <v>369</v>
-      </c>
-      <c r="V46" t="s">
-        <v>370</v>
       </c>
       <c r="W46" t="s">
         <v>371</v>
       </c>
       <c r="X46" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y46" t="s">
         <v>372</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>